<commit_message>
feat: lab3 solution in a golden ratio and web
</commit_message>
<xml_diff>
--- a/L1/task2.xlsx
+++ b/L1/task2.xlsx
@@ -107,14 +107,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="14"/>
+      <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF595959"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -172,20 +172,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -306,17 +306,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Лист1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Фьючерс на Юань (PAM3)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="5b9bd5"/>
@@ -350,7 +339,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -407,6 +395,78 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
+              <c:f>Лист1!$B$2:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0.1335</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1329</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1331</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1338</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1354</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1352</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1343</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1354</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1362</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1367</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1359</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1347</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1352</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.1352</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.1351</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.1349</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1347</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.1346</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.1348</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.1347</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Лист1!$A$2:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
@@ -437,86 +497,14 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Лист1!$B$2:$B$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
-                <c:pt idx="0">
-                  <c:v>0.1335</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.1329</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1331</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.1333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.1338</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.1354</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.1352</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.1343</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.1354</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.1362</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.1367</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.1359</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.1347</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.1352</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.1352</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.1351</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.1349</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.1347</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.1346</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.1348</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.1347</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="91832230"/>
-        <c:axId val="77246889"/>
+        <c:axId val="56728122"/>
+        <c:axId val="49579276"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91832230"/>
+        <c:axId val="56728122"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,12 +547,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77246889"/>
+        <c:crossAx val="49579276"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77246889"/>
+        <c:axId val="49579276"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -607,7 +595,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91832230"/>
+        <c:crossAx val="56728122"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -619,7 +607,7 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="span"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -680,10 +668,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0946620718756593"/>
-          <c:y val="0.157804004773903"/>
-          <c:w val="0.820521836978691"/>
-          <c:h val="0.720726694072404"/>
+          <c:x val="0.0946687297791532"/>
+          <c:y val="0.157764317180617"/>
+          <c:w val="0.820438880292587"/>
+          <c:h val="0.72067731277533"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -908,11 +896,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="9402570"/>
-        <c:axId val="62525576"/>
+        <c:axId val="87710090"/>
+        <c:axId val="3146046"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9402570"/>
+        <c:axId val="87710090"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -955,12 +943,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62525576"/>
+        <c:crossAx val="3146046"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62525576"/>
+        <c:axId val="3146046"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1003,7 +991,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9402570"/>
+        <c:crossAx val="87710090"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1267,11 +1255,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="74517700"/>
-        <c:axId val="66215076"/>
+        <c:axId val="27783014"/>
+        <c:axId val="11529858"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74517700"/>
+        <c:axId val="27783014"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1314,12 +1302,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66215076"/>
+        <c:crossAx val="11529858"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66215076"/>
+        <c:axId val="11529858"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,7 +1350,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74517700"/>
+        <c:crossAx val="27783014"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1644,11 +1632,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2225936"/>
-        <c:axId val="69686612"/>
+        <c:axId val="5472194"/>
+        <c:axId val="34287440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2225936"/>
+        <c:axId val="5472194"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1691,12 +1679,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69686612"/>
+        <c:crossAx val="34287440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69686612"/>
+        <c:axId val="34287440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1739,7 +1727,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2225936"/>
+        <c:crossAx val="5472194"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1778,9 +1766,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>357840</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>198720</xdr:rowOff>
+      <xdr:colOff>357480</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1789,7 +1777,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3913920" y="41760"/>
-        <a:ext cx="5118480" cy="2723760"/>
+        <a:ext cx="5118120" cy="2723400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1804,13 +1792,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>7560</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>83880</xdr:rowOff>
+      <xdr:rowOff>191160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>312120</xdr:colOff>
+      <xdr:colOff>311760</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>117720</xdr:rowOff>
+      <xdr:rowOff>153000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1819,7 +1807,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3868200" y="3050640"/>
-        <a:ext cx="5118480" cy="2615040"/>
+        <a:ext cx="5118120" cy="2614680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1834,13 +1822,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>541080</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>198720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>235440</xdr:colOff>
+      <xdr:colOff>235080</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1849,7 +1837,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9215640" y="3058200"/>
-        <a:ext cx="5196240" cy="2714400"/>
+        <a:ext cx="5195880" cy="2714040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1868,9 +1856,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>335880</xdr:colOff>
+      <xdr:colOff>335520</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>9720</xdr:rowOff>
+      <xdr:rowOff>124920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1879,7 +1867,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="9393840" y="61920"/>
-        <a:ext cx="5118480" cy="2714400"/>
+        <a:ext cx="5118120" cy="2714040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2069,195 +2057,194 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="123" zoomScaleNormal="123" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L35" activeCellId="0" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.44"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="4" t="n">
         <v>0.1335</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
         <v>0.1329</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="4" t="n">
         <v>0.1331</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
+    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
         <v>45202</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="4" t="n">
         <v>0.1333</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
         <v>45172</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="4" t="n">
         <v>0.1338</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
         <v>45141</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="4" t="n">
         <v>0.1354</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
         <v>45110</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="4" t="n">
         <v>0.1352</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
         <v>45080</v>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B9" s="4" t="n">
         <v>0.1343</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
         <v>44988</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="4" t="n">
         <v>0.1354</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
         <v>44960</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="4" t="n">
         <v>0.1362</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+    <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="n">
         <v>44929</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="4" t="n">
         <v>0.1367</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+    <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="4" t="n">
         <v>0.1359</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+    <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="4" t="n">
         <v>0.1347</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="4" t="n">
         <v>0.1352</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="4" t="n">
         <v>0.1352</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+    <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="4" t="n">
         <v>0.1351</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+    <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="3" t="n">
+      <c r="B18" s="4" t="n">
         <v>0.1349</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="3" t="n">
+      <c r="B19" s="4" t="n">
         <v>0.1347</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="4" t="n">
         <v>0.1346</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+    <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="4" t="n">
         <v>0.1348</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+    <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="4" t="n">
         <v>0.1347</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>